<commit_message>
cambios en PC Gestion Documental para guardar en R
</commit_message>
<xml_diff>
--- a/Sura/DataSource  - Endoso Exclusión de Riesgo.xlsx
+++ b/Sura/DataSource  - Endoso Exclusión de Riesgo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B32713BA-DC70-431D-A4BE-AB0948603424}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DF7E22-C6D5-4302-978A-EC0EF2F72C11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BD215C97-67FE-4B28-84C1-B2C2E020DEBB}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>gw</t>
   </si>
   <si>
-    <t>04104013802</t>
-  </si>
-  <si>
     <t>Exclusión de Riesgo</t>
+  </si>
+  <si>
+    <t>04104016708</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +473,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>